<commit_message>
Update graphical overview and readme
</commit_message>
<xml_diff>
--- a/documents/GraphicalOverview.xlsx
+++ b/documents/GraphicalOverview.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
   <si>
     <t>Byte Number</t>
   </si>
@@ -41,9 +41,6 @@
     <t>noOfFirstLog</t>
   </si>
   <si>
-    <t>noOfCurrentLog</t>
-  </si>
-  <si>
     <t>long 1</t>
   </si>
   <si>
@@ -65,38 +62,10 @@
     <t>LOG NUMBER 1</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>EEPROM - LOGGER</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">the logger manages the logs </t>
-    </r>
+    <t>noOfNextLog</t>
+  </si>
+  <si>
+    <t>…</t>
   </si>
   <si>
     <r>
@@ -129,7 +98,41 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>the counter manages the storage of the values on the the EEPROM</t>
+      <t>the counter is used as storage manager for the EEPROM memory, it works with long values</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>EEPROM - LOGGER</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+t</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">he logger gets logs from the main programm, converts them to longs, and passes them on to the eeprom-counter and vice versa </t>
     </r>
   </si>
 </sst>
@@ -246,7 +249,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -285,100 +288,55 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
@@ -464,6 +422,118 @@
         <color indexed="64"/>
       </right>
       <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -475,7 +545,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -489,125 +559,155 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1170,106 +1270,113 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F12:Y21"/>
+  <dimension ref="F12:AA21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="11.42578125" style="2"/>
-    <col min="6" max="9" width="5.85546875" style="2" customWidth="1"/>
-    <col min="10" max="25" width="4.140625" style="2" customWidth="1"/>
-    <col min="26" max="16384" width="11.42578125" style="2"/>
+    <col min="6" max="26" width="5" style="2" customWidth="1"/>
+    <col min="27" max="27" width="11.42578125" style="45"/>
+    <col min="28" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="12" spans="6:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="6:25" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F13" s="43" t="s">
+    <row r="12" spans="6:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="6:26" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="50"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="50"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="50"/>
+      <c r="M13" s="50"/>
+      <c r="N13" s="50"/>
+      <c r="O13" s="50"/>
+      <c r="P13" s="50"/>
+      <c r="Q13" s="50"/>
+      <c r="R13" s="50"/>
+      <c r="S13" s="50"/>
+      <c r="T13" s="50"/>
+      <c r="U13" s="50"/>
+      <c r="V13" s="50"/>
+      <c r="W13" s="50"/>
+      <c r="X13" s="50"/>
+      <c r="Y13" s="50"/>
+      <c r="Z13" s="51"/>
+    </row>
+    <row r="14" spans="6:26" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F14" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="39"/>
+      <c r="R14" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="S14" s="10"/>
+      <c r="T14" s="10"/>
+      <c r="U14" s="10"/>
+      <c r="V14" s="10"/>
+      <c r="W14" s="10"/>
+      <c r="X14" s="10"/>
+      <c r="Y14" s="43"/>
+      <c r="Z14" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="41"/>
-      <c r="J13" s="41"/>
-      <c r="K13" s="41"/>
-      <c r="L13" s="41"/>
-      <c r="M13" s="41"/>
-      <c r="N13" s="41"/>
-      <c r="O13" s="41"/>
-      <c r="P13" s="41"/>
-      <c r="Q13" s="41"/>
-      <c r="R13" s="41"/>
-      <c r="S13" s="41"/>
-      <c r="T13" s="41"/>
-      <c r="U13" s="41"/>
-      <c r="V13" s="41"/>
-      <c r="W13" s="41"/>
-      <c r="X13" s="41"/>
-      <c r="Y13" s="42"/>
     </row>
-    <row r="14" spans="6:25" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F14" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="K14" s="33"/>
-      <c r="L14" s="33"/>
-      <c r="M14" s="33"/>
-      <c r="N14" s="33"/>
-      <c r="O14" s="33"/>
-      <c r="P14" s="33"/>
-      <c r="Q14" s="34"/>
-      <c r="R14" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="S14" s="9"/>
-      <c r="T14" s="9"/>
-      <c r="U14" s="9"/>
-      <c r="V14" s="9"/>
-      <c r="W14" s="9"/>
-      <c r="X14" s="9"/>
-      <c r="Y14" s="10"/>
+    <row r="15" spans="6:26" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F15" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="O15" s="23"/>
+      <c r="P15" s="23"/>
+      <c r="Q15" s="40"/>
+      <c r="R15" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="S15" s="23"/>
+      <c r="T15" s="23"/>
+      <c r="U15" s="23"/>
+      <c r="V15" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="W15" s="23"/>
+      <c r="X15" s="23"/>
+      <c r="Y15" s="40"/>
+      <c r="Z15" s="44" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="15" spans="6:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F15" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="31"/>
-      <c r="J15" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="K15" s="27"/>
-      <c r="L15" s="27"/>
-      <c r="M15" s="27"/>
-      <c r="N15" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="O15" s="27"/>
-      <c r="P15" s="27"/>
-      <c r="Q15" s="28"/>
-      <c r="R15" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="S15" s="27"/>
-      <c r="T15" s="27"/>
-      <c r="U15" s="27"/>
-      <c r="V15" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="W15" s="27"/>
-      <c r="X15" s="27"/>
-      <c r="Y15" s="28"/>
-    </row>
-    <row r="16" spans="6:25" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="6:26" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F16" s="3">
         <v>1</v>
       </c>
@@ -1279,7 +1386,7 @@
       <c r="H16" s="4">
         <v>3</v>
       </c>
-      <c r="I16" s="5">
+      <c r="I16" s="33">
         <v>4</v>
       </c>
       <c r="J16" s="3">
@@ -1303,7 +1410,7 @@
       <c r="P16" s="4">
         <v>3</v>
       </c>
-      <c r="Q16" s="5">
+      <c r="Q16" s="33">
         <v>4</v>
       </c>
       <c r="R16" s="3">
@@ -1327,186 +1434,202 @@
       <c r="X16" s="4">
         <v>3</v>
       </c>
-      <c r="Y16" s="5">
+      <c r="Y16" s="33">
         <v>4</v>
       </c>
+      <c r="Z16" s="44" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="17" spans="6:25" s="1" customFormat="1" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F17" s="35" t="s">
+    <row r="17" spans="6:27" s="1" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F17" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="G17" s="36"/>
-      <c r="H17" s="37" t="s">
+      <c r="G17" s="26"/>
+      <c r="H17" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" s="34"/>
+      <c r="J17" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="K17" s="36"/>
+      <c r="L17" s="36"/>
+      <c r="M17" s="36"/>
+      <c r="N17" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="O17" s="37"/>
+      <c r="P17" s="37"/>
+      <c r="Q17" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="R17" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="S17" s="36"/>
+      <c r="T17" s="36"/>
+      <c r="U17" s="36"/>
+      <c r="V17" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="W17" s="37"/>
+      <c r="X17" s="37"/>
+      <c r="Y17" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z17" s="54" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA17" s="46"/>
+    </row>
+    <row r="18" spans="6:27" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F18" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
+      <c r="N18" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="O18" s="30"/>
+      <c r="P18" s="30"/>
+      <c r="Q18" s="35"/>
+      <c r="R18" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="S18" s="20"/>
+      <c r="T18" s="20"/>
+      <c r="U18" s="20"/>
+      <c r="V18" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="W18" s="30"/>
+      <c r="X18" s="30"/>
+      <c r="Y18" s="35"/>
+      <c r="Z18" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA18" s="46"/>
+    </row>
+    <row r="19" spans="6:27" s="1" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="5"/>
+      <c r="U19" s="5"/>
+      <c r="V19" s="5"/>
+      <c r="W19" s="5"/>
+      <c r="X19" s="5"/>
+      <c r="Y19" s="5"/>
+      <c r="AA19" s="46"/>
+    </row>
+    <row r="20" spans="6:27" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F20" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="47"/>
+      <c r="H20" s="47"/>
+      <c r="I20" s="47"/>
+      <c r="J20" s="47"/>
+      <c r="K20" s="47"/>
+      <c r="L20" s="47"/>
+      <c r="M20" s="47"/>
+      <c r="N20" s="47"/>
+      <c r="O20" s="47"/>
+      <c r="P20" s="47"/>
+      <c r="Q20" s="47"/>
+      <c r="R20" s="47"/>
+      <c r="S20" s="47"/>
+      <c r="T20" s="47"/>
+      <c r="U20" s="47"/>
+      <c r="V20" s="47"/>
+      <c r="W20" s="47"/>
+      <c r="X20" s="47"/>
+      <c r="Y20" s="47"/>
+      <c r="Z20" s="48"/>
+    </row>
+    <row r="21" spans="6:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F21" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="I17" s="38"/>
-      <c r="J17" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
-      <c r="M17" s="19"/>
-      <c r="N17" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="O17" s="17"/>
-      <c r="P17" s="17"/>
-      <c r="Q17" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="R17" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="S17" s="19"/>
-      <c r="T17" s="19"/>
-      <c r="U17" s="19"/>
-      <c r="V17" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="W17" s="17"/>
-      <c r="X17" s="17"/>
-      <c r="Y17" s="7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="6:25" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="K18" s="21"/>
-      <c r="L18" s="21"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="O18" s="24"/>
-      <c r="P18" s="24"/>
-      <c r="Q18" s="25"/>
-      <c r="R18" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="S18" s="21"/>
-      <c r="T18" s="21"/>
-      <c r="U18" s="22"/>
-      <c r="V18" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="W18" s="24"/>
-      <c r="X18" s="24"/>
-      <c r="Y18" s="25"/>
-    </row>
-    <row r="19" spans="6:25" s="1" customFormat="1" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="6"/>
-      <c r="Q19" s="6"/>
-      <c r="R19" s="6"/>
-      <c r="S19" s="6"/>
-      <c r="T19" s="6"/>
-      <c r="U19" s="6"/>
-      <c r="V19" s="6"/>
-      <c r="W19" s="6"/>
-      <c r="X19" s="6"/>
-      <c r="Y19" s="6"/>
-    </row>
-    <row r="20" spans="6:25" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F20" s="44" t="s">
-        <v>17</v>
-      </c>
-      <c r="G20" s="39"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
-      <c r="K20" s="39"/>
-      <c r="L20" s="39"/>
-      <c r="M20" s="39"/>
-      <c r="N20" s="39"/>
-      <c r="O20" s="39"/>
-      <c r="P20" s="39"/>
-      <c r="Q20" s="39"/>
-      <c r="R20" s="39"/>
-      <c r="S20" s="39"/>
-      <c r="T20" s="39"/>
-      <c r="U20" s="39"/>
-      <c r="V20" s="39"/>
-      <c r="W20" s="39"/>
-      <c r="X20" s="39"/>
-      <c r="Y20" s="40"/>
-    </row>
-    <row r="21" spans="6:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F21" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G21" s="15"/>
-      <c r="H21" s="15"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="11" t="s">
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="O21" s="17"/>
+      <c r="P21" s="17"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="O21" s="15"/>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="16"/>
-      <c r="R21" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="S21" s="12"/>
-      <c r="T21" s="12"/>
-      <c r="U21" s="13"/>
-      <c r="V21" s="14" t="s">
+      <c r="S21" s="14"/>
+      <c r="T21" s="14"/>
+      <c r="U21" s="15"/>
+      <c r="V21" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="W21" s="15"/>
-      <c r="X21" s="15"/>
-      <c r="Y21" s="16"/>
+      <c r="W21" s="17"/>
+      <c r="X21" s="17"/>
+      <c r="Y21" s="42"/>
+      <c r="Z21" s="49" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="F13:Y13"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="N17:P17"/>
-    <mergeCell ref="J14:Q14"/>
+    <mergeCell ref="R21:U21"/>
+    <mergeCell ref="V21:Y21"/>
+    <mergeCell ref="V17:X17"/>
+    <mergeCell ref="R17:U17"/>
+    <mergeCell ref="J18:M18"/>
+    <mergeCell ref="N18:Q18"/>
+    <mergeCell ref="R18:U18"/>
+    <mergeCell ref="V18:Y18"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="F20:Z20"/>
     <mergeCell ref="J21:M21"/>
     <mergeCell ref="N21:Q21"/>
     <mergeCell ref="J17:M17"/>
     <mergeCell ref="F17:G17"/>
     <mergeCell ref="H17:I17"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="N17:P17"/>
+    <mergeCell ref="J14:Q14"/>
     <mergeCell ref="R14:Y14"/>
-    <mergeCell ref="R21:U21"/>
-    <mergeCell ref="V21:Y21"/>
-    <mergeCell ref="V17:X17"/>
-    <mergeCell ref="R17:U17"/>
-    <mergeCell ref="F20:Y20"/>
-    <mergeCell ref="J18:M18"/>
-    <mergeCell ref="N18:Q18"/>
-    <mergeCell ref="R18:U18"/>
-    <mergeCell ref="V18:Y18"/>
     <mergeCell ref="J15:M15"/>
     <mergeCell ref="N15:Q15"/>
     <mergeCell ref="R15:U15"/>
     <mergeCell ref="V15:Y15"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="F13:Z13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>